<commit_message>
Formateado mejor el nombre de evento
</commit_message>
<xml_diff>
--- a/TP FINAL.xlsx
+++ b/TP FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Contenidos\Santi\UTN\4to_año\SIM\Simulacion-Final-UTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57628466-63CC-4814-B188-197335465F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A53E11-92E3-41BB-A595-F824508C8A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13320" yWindow="1380" windowWidth="12840" windowHeight="12405" xr2:uid="{EB645DF0-4BF5-4302-9DAF-5E20BFDBC0B8}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362D168F-672D-4500-A6A6-E89EE5BA079A}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W13" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>